<commit_message>
Updates to the Latest Packages
- Updates to the latest versions of existing packages
</commit_message>
<xml_diff>
--- a/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
+++ b/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dboskovic/Code/platform-sdk-mono/packages/plugin-xlsx-extractor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{577314ED-3619-5941-87C8-875029CA835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="5280" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Rebates-Purchases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="228">
   <si>
     <t>notdata</t>
   </si>
@@ -676,6 +677,51 @@
   </si>
   <si>
     <t>47123y14huh912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Group*</t>
+  </si>
+  <si>
+    <t>Rebates</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>David Johnson</t>
+  </si>
+  <si>
+    <t>Group C</t>
+  </si>
+  <si>
+    <t>Lisa Adams</t>
+  </si>
+  <si>
+    <t>Group D</t>
+  </si>
+  <si>
+    <t>Mary Johnson</t>
+  </si>
+  <si>
+    <t>Group E</t>
   </si>
 </sst>
 </file>
@@ -750,12 +796,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,11 +1120,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1113,12 +1159,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1140,120 +1191,120 @@
     <col min="1" max="26" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:61" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1300,7 +1351,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>11977</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1403,7 +1454,7 @@
         <v>45</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>16757</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -1504,7 +1555,7 @@
         <v>45</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>16757</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -1607,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>11161</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1710,7 +1761,7 @@
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>11963</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -1813,7 +1864,7 @@
         <v>45</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>13715</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1916,7 +1967,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>11011</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -2019,7 +2070,7 @@
         <v>45</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>17759</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2122,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>10617</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -2225,7 +2276,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>10451</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -2328,7 +2379,7 @@
         <v>45</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>13105</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -2431,7 +2482,7 @@
         <v>45</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>17110</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -2534,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>13806</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2637,7 +2688,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>15820</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -2740,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>10031</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -2843,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>9891</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2946,7 +2997,7 @@
         <v>45</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>14028</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -3049,7 +3100,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>10608</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -3152,7 +3203,7 @@
         <v>45</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>13905</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -3255,7 +3306,7 @@
         <v>45</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <v>20820</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -3358,7 +3409,7 @@
         <v>45</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <v>13829</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -3461,7 +3512,7 @@
         <v>45</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>10562</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -3564,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>12853</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -3667,7 +3718,7 @@
         <v>45</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <v>12241</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -3770,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <v>9759</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -3873,7 +3924,7 @@
         <v>45</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <v>9544</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -3976,7 +4027,7 @@
         <v>45</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <v>9082</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -4079,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <v>8522</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -4182,7 +4233,7 @@
         <v>45</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>12653</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -4274,4 +4325,576 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="D1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="E1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="F1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="G1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="H1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="I1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="J1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="K1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="L1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="M1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="N1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="O1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="P1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="R1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="S1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="T1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="U1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="V1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="W1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="X1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>45283</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R2" t="s">
+        <v>217</v>
+      </c>
+      <c r="S2" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" t="s">
+        <v>216</v>
+      </c>
+      <c r="V2" t="s">
+        <v>217</v>
+      </c>
+      <c r="W2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>1100</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>1200</v>
+      </c>
+      <c r="I3">
+        <v>130</v>
+      </c>
+      <c r="J3">
+        <v>1300</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+      <c r="L3">
+        <v>1400</v>
+      </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="N3">
+        <v>1500</v>
+      </c>
+      <c r="O3">
+        <v>160</v>
+      </c>
+      <c r="P3">
+        <v>1600</v>
+      </c>
+      <c r="Q3">
+        <v>170</v>
+      </c>
+      <c r="R3">
+        <v>1700</v>
+      </c>
+      <c r="S3">
+        <v>180</v>
+      </c>
+      <c r="T3">
+        <v>1800</v>
+      </c>
+      <c r="U3">
+        <v>190</v>
+      </c>
+      <c r="V3">
+        <v>1900</v>
+      </c>
+      <c r="W3">
+        <v>200</v>
+      </c>
+      <c r="X3">
+        <v>2000</v>
+      </c>
+      <c r="Y3">
+        <v>210</v>
+      </c>
+      <c r="Z3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="F4">
+        <v>2100</v>
+      </c>
+      <c r="G4">
+        <v>220</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>2300</v>
+      </c>
+      <c r="K4">
+        <v>240</v>
+      </c>
+      <c r="L4">
+        <v>2400</v>
+      </c>
+      <c r="M4">
+        <v>250</v>
+      </c>
+      <c r="N4">
+        <v>2500</v>
+      </c>
+      <c r="O4">
+        <v>260</v>
+      </c>
+      <c r="P4">
+        <v>2600</v>
+      </c>
+      <c r="Q4">
+        <v>270</v>
+      </c>
+      <c r="R4">
+        <v>2700</v>
+      </c>
+      <c r="S4">
+        <v>280</v>
+      </c>
+      <c r="T4">
+        <v>2800</v>
+      </c>
+      <c r="U4">
+        <v>290</v>
+      </c>
+      <c r="V4">
+        <v>2900</v>
+      </c>
+      <c r="W4">
+        <v>300</v>
+      </c>
+      <c r="X4">
+        <v>3000</v>
+      </c>
+      <c r="Y4">
+        <v>310</v>
+      </c>
+      <c r="Z4">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5">
+        <v>310</v>
+      </c>
+      <c r="F5">
+        <v>3100</v>
+      </c>
+      <c r="G5">
+        <v>320</v>
+      </c>
+      <c r="H5">
+        <v>3200</v>
+      </c>
+      <c r="I5">
+        <v>330</v>
+      </c>
+      <c r="J5">
+        <v>3300</v>
+      </c>
+      <c r="K5">
+        <v>340</v>
+      </c>
+      <c r="L5">
+        <v>3400</v>
+      </c>
+      <c r="M5">
+        <v>350</v>
+      </c>
+      <c r="N5">
+        <v>3500</v>
+      </c>
+      <c r="O5">
+        <v>360</v>
+      </c>
+      <c r="P5">
+        <v>3600</v>
+      </c>
+      <c r="Q5">
+        <v>370</v>
+      </c>
+      <c r="R5">
+        <v>3700</v>
+      </c>
+      <c r="S5">
+        <v>380</v>
+      </c>
+      <c r="T5">
+        <v>3800</v>
+      </c>
+      <c r="U5">
+        <v>390</v>
+      </c>
+      <c r="V5">
+        <v>3900</v>
+      </c>
+      <c r="W5">
+        <v>400</v>
+      </c>
+      <c r="X5">
+        <v>4000</v>
+      </c>
+      <c r="Y5">
+        <v>410</v>
+      </c>
+      <c r="Z5">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6">
+        <v>410</v>
+      </c>
+      <c r="F6">
+        <v>4100</v>
+      </c>
+      <c r="G6">
+        <v>420</v>
+      </c>
+      <c r="H6">
+        <v>4200</v>
+      </c>
+      <c r="I6">
+        <v>430</v>
+      </c>
+      <c r="J6">
+        <v>4300</v>
+      </c>
+      <c r="K6">
+        <v>440</v>
+      </c>
+      <c r="L6">
+        <v>4400</v>
+      </c>
+      <c r="M6">
+        <v>450</v>
+      </c>
+      <c r="N6">
+        <v>4500</v>
+      </c>
+      <c r="O6">
+        <v>460</v>
+      </c>
+      <c r="P6">
+        <v>4600</v>
+      </c>
+      <c r="Q6">
+        <v>470</v>
+      </c>
+      <c r="R6">
+        <v>4700</v>
+      </c>
+      <c r="S6">
+        <v>480</v>
+      </c>
+      <c r="T6">
+        <v>4800</v>
+      </c>
+      <c r="U6">
+        <v>490</v>
+      </c>
+      <c r="V6">
+        <v>4900</v>
+      </c>
+      <c r="W6">
+        <v>500</v>
+      </c>
+      <c r="X6">
+        <v>5000</v>
+      </c>
+      <c r="Y6">
+        <v>510</v>
+      </c>
+      <c r="Z6">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>510</v>
+      </c>
+      <c r="F7">
+        <v>5100</v>
+      </c>
+      <c r="G7">
+        <v>520</v>
+      </c>
+      <c r="H7">
+        <v>5200</v>
+      </c>
+      <c r="I7">
+        <v>530</v>
+      </c>
+      <c r="J7">
+        <v>5300</v>
+      </c>
+      <c r="K7">
+        <v>540</v>
+      </c>
+      <c r="L7">
+        <v>5400</v>
+      </c>
+      <c r="M7">
+        <v>550</v>
+      </c>
+      <c r="N7">
+        <v>5500</v>
+      </c>
+      <c r="O7">
+        <v>560</v>
+      </c>
+      <c r="P7">
+        <v>5600</v>
+      </c>
+      <c r="Q7">
+        <v>570</v>
+      </c>
+      <c r="R7">
+        <v>5700</v>
+      </c>
+      <c r="S7">
+        <v>580</v>
+      </c>
+      <c r="T7">
+        <v>5800</v>
+      </c>
+      <c r="U7">
+        <v>590</v>
+      </c>
+      <c r="V7">
+        <v>5900</v>
+      </c>
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7">
+        <v>6000</v>
+      </c>
+      <c r="Y7">
+        <v>610</v>
+      </c>
+      <c r="Z7">
+        <v>6100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Updates to the Latest Packages"
This reverts commit 251230b75dc9a9f0d5e70ff4fc036ef02e366a8a.
</commit_message>
<xml_diff>
--- a/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
+++ b/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dboskovic/Code/platform-sdk-mono/packages/plugin-xlsx-extractor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{577314ED-3619-5941-87C8-875029CA835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="7340" yWindow="5280" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
-    <sheet name="Rebates-Purchases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
   <si>
     <t>notdata</t>
   </si>
@@ -677,51 +676,6 @@
   </si>
   <si>
     <t>47123y14huh912</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t>Name*</t>
-  </si>
-  <si>
-    <t>Group*</t>
-  </si>
-  <si>
-    <t>Rebates</t>
-  </si>
-  <si>
-    <t>Purchases</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Group A</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>Group B</t>
-  </si>
-  <si>
-    <t>David Johnson</t>
-  </si>
-  <si>
-    <t>Group C</t>
-  </si>
-  <si>
-    <t>Lisa Adams</t>
-  </si>
-  <si>
-    <t>Group D</t>
-  </si>
-  <si>
-    <t>Mary Johnson</t>
-  </si>
-  <si>
-    <t>Group E</t>
   </si>
 </sst>
 </file>
@@ -796,12 +750,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1120,11 +1074,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1159,17 +1113,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1191,120 +1140,120 @@
     <col min="1" max="26" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:61" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="5"/>
-      <c r="AZ1" s="5"/>
-      <c r="BA1" s="5"/>
-      <c r="BB1" s="5"/>
-      <c r="BC1" s="5"/>
-      <c r="BD1" s="5"/>
-      <c r="BE1" s="5"/>
-      <c r="BF1" s="5"/>
-      <c r="BG1" s="5"/>
-      <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
+      <c r="AU1" s="6"/>
+      <c r="AV1" s="6"/>
+      <c r="AW1" s="6"/>
+      <c r="AX1" s="6"/>
+      <c r="AY1" s="6"/>
+      <c r="AZ1" s="6"/>
+      <c r="BA1" s="6"/>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="6"/>
+      <c r="BD1" s="6"/>
+      <c r="BE1" s="6"/>
+      <c r="BF1" s="6"/>
+      <c r="BG1" s="6"/>
+      <c r="BH1" s="6"/>
+      <c r="BI1" s="6"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1351,7 +1300,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="3">
+      <c r="Q2" s="4">
         <v>11977</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1454,7 +1403,7 @@
         <v>45</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3">
+      <c r="Q3" s="4">
         <v>16757</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -1555,7 +1504,7 @@
         <v>45</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3">
+      <c r="Q4" s="4">
         <v>16757</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -1658,7 +1607,7 @@
         <v>45</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3">
+      <c r="Q5" s="4">
         <v>11161</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1761,7 +1710,7 @@
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="3">
+      <c r="Q6" s="4">
         <v>11963</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -1864,7 +1813,7 @@
         <v>45</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="3">
+      <c r="Q7" s="4">
         <v>13715</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1967,7 +1916,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3">
+      <c r="Q8" s="4">
         <v>11011</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -2070,7 +2019,7 @@
         <v>45</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3">
+      <c r="Q9" s="4">
         <v>17759</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2173,7 +2122,7 @@
         <v>45</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3">
+      <c r="Q10" s="4">
         <v>10617</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -2276,7 +2225,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3">
+      <c r="Q11" s="4">
         <v>10451</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -2379,7 +2328,7 @@
         <v>45</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3">
+      <c r="Q12" s="4">
         <v>13105</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -2482,7 +2431,7 @@
         <v>45</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3">
+      <c r="Q13" s="4">
         <v>17110</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -2585,7 +2534,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3">
+      <c r="Q14" s="4">
         <v>13806</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2688,7 +2637,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3">
+      <c r="Q15" s="4">
         <v>15820</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -2791,7 +2740,7 @@
         <v>45</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="3">
+      <c r="Q16" s="4">
         <v>10031</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -2894,7 +2843,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="3">
+      <c r="Q17" s="4">
         <v>9891</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2997,7 +2946,7 @@
         <v>45</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="3">
+      <c r="Q18" s="4">
         <v>14028</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -3100,7 +3049,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="3">
+      <c r="Q19" s="4">
         <v>10608</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -3203,7 +3152,7 @@
         <v>45</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="3">
+      <c r="Q20" s="4">
         <v>13905</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -3306,7 +3255,7 @@
         <v>45</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="3">
+      <c r="Q21" s="4">
         <v>20820</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -3409,7 +3358,7 @@
         <v>45</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="3">
+      <c r="Q22" s="4">
         <v>13829</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -3512,7 +3461,7 @@
         <v>45</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="3">
+      <c r="Q23" s="4">
         <v>10562</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -3615,7 +3564,7 @@
         <v>45</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="3">
+      <c r="Q24" s="4">
         <v>12853</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -3718,7 +3667,7 @@
         <v>45</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="3">
+      <c r="Q25" s="4">
         <v>12241</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -3821,7 +3770,7 @@
         <v>45</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3">
+      <c r="Q26" s="4">
         <v>9759</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -3924,7 +3873,7 @@
         <v>45</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="3">
+      <c r="Q27" s="4">
         <v>9544</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -4027,7 +3976,7 @@
         <v>45</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="3">
+      <c r="Q28" s="4">
         <v>9082</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -4130,7 +4079,7 @@
         <v>45</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3">
+      <c r="Q29" s="4">
         <v>8522</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -4233,7 +4182,7 @@
         <v>45</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="3">
+      <c r="Q30" s="4">
         <v>12653</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -4325,576 +4274,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
-  <dimension ref="A1:Z7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C1" s="7">
-        <v>44949</v>
-      </c>
-      <c r="D1" s="7">
-        <v>44949</v>
-      </c>
-      <c r="E1" s="7">
-        <v>44980</v>
-      </c>
-      <c r="F1" s="7">
-        <v>44980</v>
-      </c>
-      <c r="G1" s="7">
-        <v>45008</v>
-      </c>
-      <c r="H1" s="7">
-        <v>45008</v>
-      </c>
-      <c r="I1" s="7">
-        <v>45039</v>
-      </c>
-      <c r="J1" s="7">
-        <v>45039</v>
-      </c>
-      <c r="K1" s="7">
-        <v>45069</v>
-      </c>
-      <c r="L1" s="7">
-        <v>45069</v>
-      </c>
-      <c r="M1" s="7">
-        <v>45100</v>
-      </c>
-      <c r="N1" s="7">
-        <v>45100</v>
-      </c>
-      <c r="O1" s="7">
-        <v>45130</v>
-      </c>
-      <c r="P1" s="7">
-        <v>45130</v>
-      </c>
-      <c r="Q1" s="7">
-        <v>45161</v>
-      </c>
-      <c r="R1" s="7">
-        <v>45161</v>
-      </c>
-      <c r="S1" s="7">
-        <v>45192</v>
-      </c>
-      <c r="T1" s="7">
-        <v>45192</v>
-      </c>
-      <c r="U1" s="7">
-        <v>45222</v>
-      </c>
-      <c r="V1" s="7">
-        <v>45222</v>
-      </c>
-      <c r="W1" s="7">
-        <v>45253</v>
-      </c>
-      <c r="X1" s="7">
-        <v>45253</v>
-      </c>
-      <c r="Y1" s="7">
-        <v>45283</v>
-      </c>
-      <c r="Z1" s="7">
-        <v>45283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" t="s">
-        <v>217</v>
-      </c>
-      <c r="M2" t="s">
-        <v>216</v>
-      </c>
-      <c r="N2" t="s">
-        <v>217</v>
-      </c>
-      <c r="O2" t="s">
-        <v>216</v>
-      </c>
-      <c r="P2" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>216</v>
-      </c>
-      <c r="R2" t="s">
-        <v>217</v>
-      </c>
-      <c r="S2" t="s">
-        <v>216</v>
-      </c>
-      <c r="T2" t="s">
-        <v>217</v>
-      </c>
-      <c r="U2" t="s">
-        <v>216</v>
-      </c>
-      <c r="V2" t="s">
-        <v>217</v>
-      </c>
-      <c r="W2" t="s">
-        <v>216</v>
-      </c>
-      <c r="X2" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>110</v>
-      </c>
-      <c r="F3">
-        <v>1100</v>
-      </c>
-      <c r="G3">
-        <v>120</v>
-      </c>
-      <c r="H3">
-        <v>1200</v>
-      </c>
-      <c r="I3">
-        <v>130</v>
-      </c>
-      <c r="J3">
-        <v>1300</v>
-      </c>
-      <c r="K3">
-        <v>140</v>
-      </c>
-      <c r="L3">
-        <v>1400</v>
-      </c>
-      <c r="M3">
-        <v>150</v>
-      </c>
-      <c r="N3">
-        <v>1500</v>
-      </c>
-      <c r="O3">
-        <v>160</v>
-      </c>
-      <c r="P3">
-        <v>1600</v>
-      </c>
-      <c r="Q3">
-        <v>170</v>
-      </c>
-      <c r="R3">
-        <v>1700</v>
-      </c>
-      <c r="S3">
-        <v>180</v>
-      </c>
-      <c r="T3">
-        <v>1800</v>
-      </c>
-      <c r="U3">
-        <v>190</v>
-      </c>
-      <c r="V3">
-        <v>1900</v>
-      </c>
-      <c r="W3">
-        <v>200</v>
-      </c>
-      <c r="X3">
-        <v>2000</v>
-      </c>
-      <c r="Y3">
-        <v>210</v>
-      </c>
-      <c r="Z3">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>2000</v>
-      </c>
-      <c r="E4">
-        <v>210</v>
-      </c>
-      <c r="F4">
-        <v>2100</v>
-      </c>
-      <c r="G4">
-        <v>220</v>
-      </c>
-      <c r="H4">
-        <v>2200</v>
-      </c>
-      <c r="I4">
-        <v>230</v>
-      </c>
-      <c r="J4">
-        <v>2300</v>
-      </c>
-      <c r="K4">
-        <v>240</v>
-      </c>
-      <c r="L4">
-        <v>2400</v>
-      </c>
-      <c r="M4">
-        <v>250</v>
-      </c>
-      <c r="N4">
-        <v>2500</v>
-      </c>
-      <c r="O4">
-        <v>260</v>
-      </c>
-      <c r="P4">
-        <v>2600</v>
-      </c>
-      <c r="Q4">
-        <v>270</v>
-      </c>
-      <c r="R4">
-        <v>2700</v>
-      </c>
-      <c r="S4">
-        <v>280</v>
-      </c>
-      <c r="T4">
-        <v>2800</v>
-      </c>
-      <c r="U4">
-        <v>290</v>
-      </c>
-      <c r="V4">
-        <v>2900</v>
-      </c>
-      <c r="W4">
-        <v>300</v>
-      </c>
-      <c r="X4">
-        <v>3000</v>
-      </c>
-      <c r="Y4">
-        <v>310</v>
-      </c>
-      <c r="Z4">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="D5">
-        <v>3000</v>
-      </c>
-      <c r="E5">
-        <v>310</v>
-      </c>
-      <c r="F5">
-        <v>3100</v>
-      </c>
-      <c r="G5">
-        <v>320</v>
-      </c>
-      <c r="H5">
-        <v>3200</v>
-      </c>
-      <c r="I5">
-        <v>330</v>
-      </c>
-      <c r="J5">
-        <v>3300</v>
-      </c>
-      <c r="K5">
-        <v>340</v>
-      </c>
-      <c r="L5">
-        <v>3400</v>
-      </c>
-      <c r="M5">
-        <v>350</v>
-      </c>
-      <c r="N5">
-        <v>3500</v>
-      </c>
-      <c r="O5">
-        <v>360</v>
-      </c>
-      <c r="P5">
-        <v>3600</v>
-      </c>
-      <c r="Q5">
-        <v>370</v>
-      </c>
-      <c r="R5">
-        <v>3700</v>
-      </c>
-      <c r="S5">
-        <v>380</v>
-      </c>
-      <c r="T5">
-        <v>3800</v>
-      </c>
-      <c r="U5">
-        <v>390</v>
-      </c>
-      <c r="V5">
-        <v>3900</v>
-      </c>
-      <c r="W5">
-        <v>400</v>
-      </c>
-      <c r="X5">
-        <v>4000</v>
-      </c>
-      <c r="Y5">
-        <v>410</v>
-      </c>
-      <c r="Z5">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6">
-        <v>400</v>
-      </c>
-      <c r="D6">
-        <v>4000</v>
-      </c>
-      <c r="E6">
-        <v>410</v>
-      </c>
-      <c r="F6">
-        <v>4100</v>
-      </c>
-      <c r="G6">
-        <v>420</v>
-      </c>
-      <c r="H6">
-        <v>4200</v>
-      </c>
-      <c r="I6">
-        <v>430</v>
-      </c>
-      <c r="J6">
-        <v>4300</v>
-      </c>
-      <c r="K6">
-        <v>440</v>
-      </c>
-      <c r="L6">
-        <v>4400</v>
-      </c>
-      <c r="M6">
-        <v>450</v>
-      </c>
-      <c r="N6">
-        <v>4500</v>
-      </c>
-      <c r="O6">
-        <v>460</v>
-      </c>
-      <c r="P6">
-        <v>4600</v>
-      </c>
-      <c r="Q6">
-        <v>470</v>
-      </c>
-      <c r="R6">
-        <v>4700</v>
-      </c>
-      <c r="S6">
-        <v>480</v>
-      </c>
-      <c r="T6">
-        <v>4800</v>
-      </c>
-      <c r="U6">
-        <v>490</v>
-      </c>
-      <c r="V6">
-        <v>4900</v>
-      </c>
-      <c r="W6">
-        <v>500</v>
-      </c>
-      <c r="X6">
-        <v>5000</v>
-      </c>
-      <c r="Y6">
-        <v>510</v>
-      </c>
-      <c r="Z6">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>226</v>
-      </c>
-      <c r="B7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7">
-        <v>500</v>
-      </c>
-      <c r="D7">
-        <v>5000</v>
-      </c>
-      <c r="E7">
-        <v>510</v>
-      </c>
-      <c r="F7">
-        <v>5100</v>
-      </c>
-      <c r="G7">
-        <v>520</v>
-      </c>
-      <c r="H7">
-        <v>5200</v>
-      </c>
-      <c r="I7">
-        <v>530</v>
-      </c>
-      <c r="J7">
-        <v>5300</v>
-      </c>
-      <c r="K7">
-        <v>540</v>
-      </c>
-      <c r="L7">
-        <v>5400</v>
-      </c>
-      <c r="M7">
-        <v>550</v>
-      </c>
-      <c r="N7">
-        <v>5500</v>
-      </c>
-      <c r="O7">
-        <v>560</v>
-      </c>
-      <c r="P7">
-        <v>5600</v>
-      </c>
-      <c r="Q7">
-        <v>570</v>
-      </c>
-      <c r="R7">
-        <v>5700</v>
-      </c>
-      <c r="S7">
-        <v>580</v>
-      </c>
-      <c r="T7">
-        <v>5800</v>
-      </c>
-      <c r="U7">
-        <v>590</v>
-      </c>
-      <c r="V7">
-        <v>5900</v>
-      </c>
-      <c r="W7">
-        <v>600</v>
-      </c>
-      <c r="X7">
-        <v>6000</v>
-      </c>
-      <c r="Y7">
-        <v>610</v>
-      </c>
-      <c r="Z7">
-        <v>6100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Latest XLSX Extractor Package
- remove blank, placeholder sheet
</commit_message>
<xml_diff>
--- a/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
+++ b/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dboskovic/Code/platform-sdk-mono/packages/plugin-xlsx-extractor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{577314ED-3619-5941-87C8-875029CA835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="5280" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Rebates-Purchases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="228">
   <si>
     <t>notdata</t>
   </si>
@@ -676,6 +677,51 @@
   </si>
   <si>
     <t>47123y14huh912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Group*</t>
+  </si>
+  <si>
+    <t>Rebates</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>David Johnson</t>
+  </si>
+  <si>
+    <t>Group C</t>
+  </si>
+  <si>
+    <t>Lisa Adams</t>
+  </si>
+  <si>
+    <t>Group D</t>
+  </si>
+  <si>
+    <t>Mary Johnson</t>
+  </si>
+  <si>
+    <t>Group E</t>
   </si>
 </sst>
 </file>
@@ -750,12 +796,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,11 +1120,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1113,12 +1159,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1140,120 +1191,120 @@
     <col min="1" max="26" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:61" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1300,7 +1351,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>11977</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1403,7 +1454,7 @@
         <v>45</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>16757</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -1504,7 +1555,7 @@
         <v>45</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>16757</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -1607,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>11161</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1710,7 +1761,7 @@
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>11963</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -1813,7 +1864,7 @@
         <v>45</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>13715</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1916,7 +1967,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>11011</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -2019,7 +2070,7 @@
         <v>45</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>17759</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2122,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>10617</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -2225,7 +2276,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>10451</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -2328,7 +2379,7 @@
         <v>45</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>13105</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -2431,7 +2482,7 @@
         <v>45</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>17110</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -2534,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>13806</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2637,7 +2688,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>15820</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -2740,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>10031</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -2843,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>9891</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2946,7 +2997,7 @@
         <v>45</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>14028</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -3049,7 +3100,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>10608</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -3152,7 +3203,7 @@
         <v>45</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>13905</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -3255,7 +3306,7 @@
         <v>45</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <v>20820</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -3358,7 +3409,7 @@
         <v>45</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <v>13829</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -3461,7 +3512,7 @@
         <v>45</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>10562</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -3564,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>12853</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -3667,7 +3718,7 @@
         <v>45</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <v>12241</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -3770,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <v>9759</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -3873,7 +3924,7 @@
         <v>45</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <v>9544</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -3976,7 +4027,7 @@
         <v>45</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <v>9082</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -4079,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <v>8522</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -4182,7 +4233,7 @@
         <v>45</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>12653</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -4274,4 +4325,576 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="D1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="E1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="F1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="G1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="H1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="I1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="J1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="K1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="L1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="M1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="N1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="O1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="P1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="R1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="S1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="T1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="U1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="V1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="W1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="X1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>45283</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R2" t="s">
+        <v>217</v>
+      </c>
+      <c r="S2" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" t="s">
+        <v>216</v>
+      </c>
+      <c r="V2" t="s">
+        <v>217</v>
+      </c>
+      <c r="W2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>1100</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>1200</v>
+      </c>
+      <c r="I3">
+        <v>130</v>
+      </c>
+      <c r="J3">
+        <v>1300</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+      <c r="L3">
+        <v>1400</v>
+      </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="N3">
+        <v>1500</v>
+      </c>
+      <c r="O3">
+        <v>160</v>
+      </c>
+      <c r="P3">
+        <v>1600</v>
+      </c>
+      <c r="Q3">
+        <v>170</v>
+      </c>
+      <c r="R3">
+        <v>1700</v>
+      </c>
+      <c r="S3">
+        <v>180</v>
+      </c>
+      <c r="T3">
+        <v>1800</v>
+      </c>
+      <c r="U3">
+        <v>190</v>
+      </c>
+      <c r="V3">
+        <v>1900</v>
+      </c>
+      <c r="W3">
+        <v>200</v>
+      </c>
+      <c r="X3">
+        <v>2000</v>
+      </c>
+      <c r="Y3">
+        <v>210</v>
+      </c>
+      <c r="Z3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="F4">
+        <v>2100</v>
+      </c>
+      <c r="G4">
+        <v>220</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>2300</v>
+      </c>
+      <c r="K4">
+        <v>240</v>
+      </c>
+      <c r="L4">
+        <v>2400</v>
+      </c>
+      <c r="M4">
+        <v>250</v>
+      </c>
+      <c r="N4">
+        <v>2500</v>
+      </c>
+      <c r="O4">
+        <v>260</v>
+      </c>
+      <c r="P4">
+        <v>2600</v>
+      </c>
+      <c r="Q4">
+        <v>270</v>
+      </c>
+      <c r="R4">
+        <v>2700</v>
+      </c>
+      <c r="S4">
+        <v>280</v>
+      </c>
+      <c r="T4">
+        <v>2800</v>
+      </c>
+      <c r="U4">
+        <v>290</v>
+      </c>
+      <c r="V4">
+        <v>2900</v>
+      </c>
+      <c r="W4">
+        <v>300</v>
+      </c>
+      <c r="X4">
+        <v>3000</v>
+      </c>
+      <c r="Y4">
+        <v>310</v>
+      </c>
+      <c r="Z4">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5">
+        <v>310</v>
+      </c>
+      <c r="F5">
+        <v>3100</v>
+      </c>
+      <c r="G5">
+        <v>320</v>
+      </c>
+      <c r="H5">
+        <v>3200</v>
+      </c>
+      <c r="I5">
+        <v>330</v>
+      </c>
+      <c r="J5">
+        <v>3300</v>
+      </c>
+      <c r="K5">
+        <v>340</v>
+      </c>
+      <c r="L5">
+        <v>3400</v>
+      </c>
+      <c r="M5">
+        <v>350</v>
+      </c>
+      <c r="N5">
+        <v>3500</v>
+      </c>
+      <c r="O5">
+        <v>360</v>
+      </c>
+      <c r="P5">
+        <v>3600</v>
+      </c>
+      <c r="Q5">
+        <v>370</v>
+      </c>
+      <c r="R5">
+        <v>3700</v>
+      </c>
+      <c r="S5">
+        <v>380</v>
+      </c>
+      <c r="T5">
+        <v>3800</v>
+      </c>
+      <c r="U5">
+        <v>390</v>
+      </c>
+      <c r="V5">
+        <v>3900</v>
+      </c>
+      <c r="W5">
+        <v>400</v>
+      </c>
+      <c r="X5">
+        <v>4000</v>
+      </c>
+      <c r="Y5">
+        <v>410</v>
+      </c>
+      <c r="Z5">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6">
+        <v>410</v>
+      </c>
+      <c r="F6">
+        <v>4100</v>
+      </c>
+      <c r="G6">
+        <v>420</v>
+      </c>
+      <c r="H6">
+        <v>4200</v>
+      </c>
+      <c r="I6">
+        <v>430</v>
+      </c>
+      <c r="J6">
+        <v>4300</v>
+      </c>
+      <c r="K6">
+        <v>440</v>
+      </c>
+      <c r="L6">
+        <v>4400</v>
+      </c>
+      <c r="M6">
+        <v>450</v>
+      </c>
+      <c r="N6">
+        <v>4500</v>
+      </c>
+      <c r="O6">
+        <v>460</v>
+      </c>
+      <c r="P6">
+        <v>4600</v>
+      </c>
+      <c r="Q6">
+        <v>470</v>
+      </c>
+      <c r="R6">
+        <v>4700</v>
+      </c>
+      <c r="S6">
+        <v>480</v>
+      </c>
+      <c r="T6">
+        <v>4800</v>
+      </c>
+      <c r="U6">
+        <v>490</v>
+      </c>
+      <c r="V6">
+        <v>4900</v>
+      </c>
+      <c r="W6">
+        <v>500</v>
+      </c>
+      <c r="X6">
+        <v>5000</v>
+      </c>
+      <c r="Y6">
+        <v>510</v>
+      </c>
+      <c r="Z6">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>510</v>
+      </c>
+      <c r="F7">
+        <v>5100</v>
+      </c>
+      <c r="G7">
+        <v>520</v>
+      </c>
+      <c r="H7">
+        <v>5200</v>
+      </c>
+      <c r="I7">
+        <v>530</v>
+      </c>
+      <c r="J7">
+        <v>5300</v>
+      </c>
+      <c r="K7">
+        <v>540</v>
+      </c>
+      <c r="L7">
+        <v>5400</v>
+      </c>
+      <c r="M7">
+        <v>550</v>
+      </c>
+      <c r="N7">
+        <v>5500</v>
+      </c>
+      <c r="O7">
+        <v>560</v>
+      </c>
+      <c r="P7">
+        <v>5600</v>
+      </c>
+      <c r="Q7">
+        <v>570</v>
+      </c>
+      <c r="R7">
+        <v>5700</v>
+      </c>
+      <c r="S7">
+        <v>580</v>
+      </c>
+      <c r="T7">
+        <v>5800</v>
+      </c>
+      <c r="U7">
+        <v>590</v>
+      </c>
+      <c r="V7">
+        <v>5900</v>
+      </c>
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7">
+        <v>6000</v>
+      </c>
+      <c r="Y7">
+        <v>610</v>
+      </c>
+      <c r="Z7">
+        <v>6100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Git Ignore + Versions
 • Update git ignore to include node_modules
 • pin the versions in package.json
</commit_message>
<xml_diff>
--- a/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
+++ b/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dboskovic/Code/platform-sdk-mono/packages/plugin-xlsx-extractor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{577314ED-3619-5941-87C8-875029CA835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="5280" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Rebates-Purchases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="228">
   <si>
     <t>notdata</t>
   </si>
@@ -676,6 +677,51 @@
   </si>
   <si>
     <t>47123y14huh912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Group*</t>
+  </si>
+  <si>
+    <t>Rebates</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>David Johnson</t>
+  </si>
+  <si>
+    <t>Group C</t>
+  </si>
+  <si>
+    <t>Lisa Adams</t>
+  </si>
+  <si>
+    <t>Group D</t>
+  </si>
+  <si>
+    <t>Mary Johnson</t>
+  </si>
+  <si>
+    <t>Group E</t>
   </si>
 </sst>
 </file>
@@ -750,12 +796,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,11 +1120,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1113,12 +1159,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1140,120 +1191,120 @@
     <col min="1" max="26" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:61" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1300,7 +1351,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>11977</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1403,7 +1454,7 @@
         <v>45</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>16757</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -1504,7 +1555,7 @@
         <v>45</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>16757</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -1607,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>11161</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1710,7 +1761,7 @@
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>11963</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -1813,7 +1864,7 @@
         <v>45</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>13715</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1916,7 +1967,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>11011</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -2019,7 +2070,7 @@
         <v>45</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>17759</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2122,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>10617</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -2225,7 +2276,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>10451</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -2328,7 +2379,7 @@
         <v>45</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>13105</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -2431,7 +2482,7 @@
         <v>45</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>17110</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -2534,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>13806</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2637,7 +2688,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>15820</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -2740,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>10031</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -2843,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>9891</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2946,7 +2997,7 @@
         <v>45</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>14028</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -3049,7 +3100,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>10608</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -3152,7 +3203,7 @@
         <v>45</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>13905</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -3255,7 +3306,7 @@
         <v>45</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <v>20820</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -3358,7 +3409,7 @@
         <v>45</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <v>13829</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -3461,7 +3512,7 @@
         <v>45</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>10562</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -3564,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>12853</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -3667,7 +3718,7 @@
         <v>45</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <v>12241</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -3770,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <v>9759</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -3873,7 +3924,7 @@
         <v>45</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <v>9544</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -3976,7 +4027,7 @@
         <v>45</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <v>9082</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -4079,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <v>8522</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -4182,7 +4233,7 @@
         <v>45</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>12653</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -4274,4 +4325,576 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="D1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="E1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="F1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="G1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="H1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="I1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="J1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="K1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="L1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="M1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="N1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="O1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="P1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="R1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="S1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="T1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="U1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="V1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="W1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="X1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>45283</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R2" t="s">
+        <v>217</v>
+      </c>
+      <c r="S2" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" t="s">
+        <v>216</v>
+      </c>
+      <c r="V2" t="s">
+        <v>217</v>
+      </c>
+      <c r="W2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>1100</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>1200</v>
+      </c>
+      <c r="I3">
+        <v>130</v>
+      </c>
+      <c r="J3">
+        <v>1300</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+      <c r="L3">
+        <v>1400</v>
+      </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="N3">
+        <v>1500</v>
+      </c>
+      <c r="O3">
+        <v>160</v>
+      </c>
+      <c r="P3">
+        <v>1600</v>
+      </c>
+      <c r="Q3">
+        <v>170</v>
+      </c>
+      <c r="R3">
+        <v>1700</v>
+      </c>
+      <c r="S3">
+        <v>180</v>
+      </c>
+      <c r="T3">
+        <v>1800</v>
+      </c>
+      <c r="U3">
+        <v>190</v>
+      </c>
+      <c r="V3">
+        <v>1900</v>
+      </c>
+      <c r="W3">
+        <v>200</v>
+      </c>
+      <c r="X3">
+        <v>2000</v>
+      </c>
+      <c r="Y3">
+        <v>210</v>
+      </c>
+      <c r="Z3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="F4">
+        <v>2100</v>
+      </c>
+      <c r="G4">
+        <v>220</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>2300</v>
+      </c>
+      <c r="K4">
+        <v>240</v>
+      </c>
+      <c r="L4">
+        <v>2400</v>
+      </c>
+      <c r="M4">
+        <v>250</v>
+      </c>
+      <c r="N4">
+        <v>2500</v>
+      </c>
+      <c r="O4">
+        <v>260</v>
+      </c>
+      <c r="P4">
+        <v>2600</v>
+      </c>
+      <c r="Q4">
+        <v>270</v>
+      </c>
+      <c r="R4">
+        <v>2700</v>
+      </c>
+      <c r="S4">
+        <v>280</v>
+      </c>
+      <c r="T4">
+        <v>2800</v>
+      </c>
+      <c r="U4">
+        <v>290</v>
+      </c>
+      <c r="V4">
+        <v>2900</v>
+      </c>
+      <c r="W4">
+        <v>300</v>
+      </c>
+      <c r="X4">
+        <v>3000</v>
+      </c>
+      <c r="Y4">
+        <v>310</v>
+      </c>
+      <c r="Z4">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5">
+        <v>310</v>
+      </c>
+      <c r="F5">
+        <v>3100</v>
+      </c>
+      <c r="G5">
+        <v>320</v>
+      </c>
+      <c r="H5">
+        <v>3200</v>
+      </c>
+      <c r="I5">
+        <v>330</v>
+      </c>
+      <c r="J5">
+        <v>3300</v>
+      </c>
+      <c r="K5">
+        <v>340</v>
+      </c>
+      <c r="L5">
+        <v>3400</v>
+      </c>
+      <c r="M5">
+        <v>350</v>
+      </c>
+      <c r="N5">
+        <v>3500</v>
+      </c>
+      <c r="O5">
+        <v>360</v>
+      </c>
+      <c r="P5">
+        <v>3600</v>
+      </c>
+      <c r="Q5">
+        <v>370</v>
+      </c>
+      <c r="R5">
+        <v>3700</v>
+      </c>
+      <c r="S5">
+        <v>380</v>
+      </c>
+      <c r="T5">
+        <v>3800</v>
+      </c>
+      <c r="U5">
+        <v>390</v>
+      </c>
+      <c r="V5">
+        <v>3900</v>
+      </c>
+      <c r="W5">
+        <v>400</v>
+      </c>
+      <c r="X5">
+        <v>4000</v>
+      </c>
+      <c r="Y5">
+        <v>410</v>
+      </c>
+      <c r="Z5">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6">
+        <v>410</v>
+      </c>
+      <c r="F6">
+        <v>4100</v>
+      </c>
+      <c r="G6">
+        <v>420</v>
+      </c>
+      <c r="H6">
+        <v>4200</v>
+      </c>
+      <c r="I6">
+        <v>430</v>
+      </c>
+      <c r="J6">
+        <v>4300</v>
+      </c>
+      <c r="K6">
+        <v>440</v>
+      </c>
+      <c r="L6">
+        <v>4400</v>
+      </c>
+      <c r="M6">
+        <v>450</v>
+      </c>
+      <c r="N6">
+        <v>4500</v>
+      </c>
+      <c r="O6">
+        <v>460</v>
+      </c>
+      <c r="P6">
+        <v>4600</v>
+      </c>
+      <c r="Q6">
+        <v>470</v>
+      </c>
+      <c r="R6">
+        <v>4700</v>
+      </c>
+      <c r="S6">
+        <v>480</v>
+      </c>
+      <c r="T6">
+        <v>4800</v>
+      </c>
+      <c r="U6">
+        <v>490</v>
+      </c>
+      <c r="V6">
+        <v>4900</v>
+      </c>
+      <c r="W6">
+        <v>500</v>
+      </c>
+      <c r="X6">
+        <v>5000</v>
+      </c>
+      <c r="Y6">
+        <v>510</v>
+      </c>
+      <c r="Z6">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>510</v>
+      </c>
+      <c r="F7">
+        <v>5100</v>
+      </c>
+      <c r="G7">
+        <v>520</v>
+      </c>
+      <c r="H7">
+        <v>5200</v>
+      </c>
+      <c r="I7">
+        <v>530</v>
+      </c>
+      <c r="J7">
+        <v>5300</v>
+      </c>
+      <c r="K7">
+        <v>540</v>
+      </c>
+      <c r="L7">
+        <v>5400</v>
+      </c>
+      <c r="M7">
+        <v>550</v>
+      </c>
+      <c r="N7">
+        <v>5500</v>
+      </c>
+      <c r="O7">
+        <v>560</v>
+      </c>
+      <c r="P7">
+        <v>5600</v>
+      </c>
+      <c r="Q7">
+        <v>570</v>
+      </c>
+      <c r="R7">
+        <v>5700</v>
+      </c>
+      <c r="S7">
+        <v>580</v>
+      </c>
+      <c r="T7">
+        <v>5800</v>
+      </c>
+      <c r="U7">
+        <v>590</v>
+      </c>
+      <c r="V7">
+        <v>5900</v>
+      </c>
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7">
+        <v>6000</v>
+      </c>
+      <c r="Y7">
+        <v>610</v>
+      </c>
+      <c r="Z7">
+        <v>6100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for DCDD Validations
- Branching off specific validation work
</commit_message>
<xml_diff>
--- a/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
+++ b/node_modules/@flatfile/plugin-xlsx-extractor/ref/test-basic.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dboskovic/Code/platform-sdk-mono/packages/plugin-xlsx-extractor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{577314ED-3619-5941-87C8-875029CA835C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7340" yWindow="5280" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Rebates-Purchases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="228">
   <si>
     <t>notdata</t>
   </si>
@@ -676,6 +677,51 @@
   </si>
   <si>
     <t>47123y14huh912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Group*</t>
+  </si>
+  <si>
+    <t>Rebates</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>David Johnson</t>
+  </si>
+  <si>
+    <t>Group C</t>
+  </si>
+  <si>
+    <t>Lisa Adams</t>
+  </si>
+  <si>
+    <t>Group D</t>
+  </si>
+  <si>
+    <t>Mary Johnson</t>
+  </si>
+  <si>
+    <t>Group E</t>
   </si>
 </sst>
 </file>
@@ -750,12 +796,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1074,11 +1120,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1113,12 +1159,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1140,120 +1191,120 @@
     <col min="1" max="26" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:61" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1300,7 +1351,7 @@
         <v>45</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>11977</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -1403,7 +1454,7 @@
         <v>45</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>16757</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -1504,7 +1555,7 @@
         <v>45</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>16757</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -1607,7 +1658,7 @@
         <v>45</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>11161</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1710,7 +1761,7 @@
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>11963</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -1813,7 +1864,7 @@
         <v>45</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>13715</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -1916,7 +1967,7 @@
         <v>45</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>11011</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -2019,7 +2070,7 @@
         <v>45</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>17759</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -2122,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>10617</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -2225,7 +2276,7 @@
         <v>45</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>10451</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -2328,7 +2379,7 @@
         <v>45</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>13105</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -2431,7 +2482,7 @@
         <v>45</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>17110</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -2534,7 +2585,7 @@
         <v>45</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>13806</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -2637,7 +2688,7 @@
         <v>45</v>
       </c>
       <c r="P15" s="3"/>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>15820</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -2740,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>10031</v>
       </c>
       <c r="R16" s="3" t="s">
@@ -2843,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>9891</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2946,7 +2997,7 @@
         <v>45</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>14028</v>
       </c>
       <c r="R18" s="3" t="s">
@@ -3049,7 +3100,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>10608</v>
       </c>
       <c r="R19" s="3" t="s">
@@ -3152,7 +3203,7 @@
         <v>45</v>
       </c>
       <c r="P20" s="3"/>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>13905</v>
       </c>
       <c r="R20" s="3" t="s">
@@ -3255,7 +3306,7 @@
         <v>45</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <v>20820</v>
       </c>
       <c r="R21" s="3" t="s">
@@ -3358,7 +3409,7 @@
         <v>45</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <v>13829</v>
       </c>
       <c r="R22" s="3" t="s">
@@ -3461,7 +3512,7 @@
         <v>45</v>
       </c>
       <c r="P23" s="3"/>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>10562</v>
       </c>
       <c r="R23" s="3" t="s">
@@ -3564,7 +3615,7 @@
         <v>45</v>
       </c>
       <c r="P24" s="3"/>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>12853</v>
       </c>
       <c r="R24" s="3" t="s">
@@ -3667,7 +3718,7 @@
         <v>45</v>
       </c>
       <c r="P25" s="3"/>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <v>12241</v>
       </c>
       <c r="R25" s="3" t="s">
@@ -3770,7 +3821,7 @@
         <v>45</v>
       </c>
       <c r="P26" s="3"/>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <v>9759</v>
       </c>
       <c r="R26" s="3" t="s">
@@ -3873,7 +3924,7 @@
         <v>45</v>
       </c>
       <c r="P27" s="3"/>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <v>9544</v>
       </c>
       <c r="R27" s="3" t="s">
@@ -3976,7 +4027,7 @@
         <v>45</v>
       </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <v>9082</v>
       </c>
       <c r="R28" s="3" t="s">
@@ -4079,7 +4130,7 @@
         <v>45</v>
       </c>
       <c r="P29" s="3"/>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <v>8522</v>
       </c>
       <c r="R29" s="3" t="s">
@@ -4182,7 +4233,7 @@
         <v>45</v>
       </c>
       <c r="P30" s="3"/>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>12653</v>
       </c>
       <c r="R30" s="3" t="s">
@@ -4274,4 +4325,576 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
+  <dimension ref="A1:Z7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="D1" s="7">
+        <v>44949</v>
+      </c>
+      <c r="E1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="F1" s="7">
+        <v>44980</v>
+      </c>
+      <c r="G1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="H1" s="7">
+        <v>45008</v>
+      </c>
+      <c r="I1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="J1" s="7">
+        <v>45039</v>
+      </c>
+      <c r="K1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="L1" s="7">
+        <v>45069</v>
+      </c>
+      <c r="M1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="N1" s="7">
+        <v>45100</v>
+      </c>
+      <c r="O1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="P1" s="7">
+        <v>45130</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="R1" s="7">
+        <v>45161</v>
+      </c>
+      <c r="S1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="T1" s="7">
+        <v>45192</v>
+      </c>
+      <c r="U1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="V1" s="7">
+        <v>45222</v>
+      </c>
+      <c r="W1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="X1" s="7">
+        <v>45253</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>45283</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" t="s">
+        <v>217</v>
+      </c>
+      <c r="O2" t="s">
+        <v>216</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>216</v>
+      </c>
+      <c r="R2" t="s">
+        <v>217</v>
+      </c>
+      <c r="S2" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" t="s">
+        <v>216</v>
+      </c>
+      <c r="V2" t="s">
+        <v>217</v>
+      </c>
+      <c r="W2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>1100</v>
+      </c>
+      <c r="G3">
+        <v>120</v>
+      </c>
+      <c r="H3">
+        <v>1200</v>
+      </c>
+      <c r="I3">
+        <v>130</v>
+      </c>
+      <c r="J3">
+        <v>1300</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+      <c r="L3">
+        <v>1400</v>
+      </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="N3">
+        <v>1500</v>
+      </c>
+      <c r="O3">
+        <v>160</v>
+      </c>
+      <c r="P3">
+        <v>1600</v>
+      </c>
+      <c r="Q3">
+        <v>170</v>
+      </c>
+      <c r="R3">
+        <v>1700</v>
+      </c>
+      <c r="S3">
+        <v>180</v>
+      </c>
+      <c r="T3">
+        <v>1800</v>
+      </c>
+      <c r="U3">
+        <v>190</v>
+      </c>
+      <c r="V3">
+        <v>1900</v>
+      </c>
+      <c r="W3">
+        <v>200</v>
+      </c>
+      <c r="X3">
+        <v>2000</v>
+      </c>
+      <c r="Y3">
+        <v>210</v>
+      </c>
+      <c r="Z3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>210</v>
+      </c>
+      <c r="F4">
+        <v>2100</v>
+      </c>
+      <c r="G4">
+        <v>220</v>
+      </c>
+      <c r="H4">
+        <v>2200</v>
+      </c>
+      <c r="I4">
+        <v>230</v>
+      </c>
+      <c r="J4">
+        <v>2300</v>
+      </c>
+      <c r="K4">
+        <v>240</v>
+      </c>
+      <c r="L4">
+        <v>2400</v>
+      </c>
+      <c r="M4">
+        <v>250</v>
+      </c>
+      <c r="N4">
+        <v>2500</v>
+      </c>
+      <c r="O4">
+        <v>260</v>
+      </c>
+      <c r="P4">
+        <v>2600</v>
+      </c>
+      <c r="Q4">
+        <v>270</v>
+      </c>
+      <c r="R4">
+        <v>2700</v>
+      </c>
+      <c r="S4">
+        <v>280</v>
+      </c>
+      <c r="T4">
+        <v>2800</v>
+      </c>
+      <c r="U4">
+        <v>290</v>
+      </c>
+      <c r="V4">
+        <v>2900</v>
+      </c>
+      <c r="W4">
+        <v>300</v>
+      </c>
+      <c r="X4">
+        <v>3000</v>
+      </c>
+      <c r="Y4">
+        <v>310</v>
+      </c>
+      <c r="Z4">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5">
+        <v>310</v>
+      </c>
+      <c r="F5">
+        <v>3100</v>
+      </c>
+      <c r="G5">
+        <v>320</v>
+      </c>
+      <c r="H5">
+        <v>3200</v>
+      </c>
+      <c r="I5">
+        <v>330</v>
+      </c>
+      <c r="J5">
+        <v>3300</v>
+      </c>
+      <c r="K5">
+        <v>340</v>
+      </c>
+      <c r="L5">
+        <v>3400</v>
+      </c>
+      <c r="M5">
+        <v>350</v>
+      </c>
+      <c r="N5">
+        <v>3500</v>
+      </c>
+      <c r="O5">
+        <v>360</v>
+      </c>
+      <c r="P5">
+        <v>3600</v>
+      </c>
+      <c r="Q5">
+        <v>370</v>
+      </c>
+      <c r="R5">
+        <v>3700</v>
+      </c>
+      <c r="S5">
+        <v>380</v>
+      </c>
+      <c r="T5">
+        <v>3800</v>
+      </c>
+      <c r="U5">
+        <v>390</v>
+      </c>
+      <c r="V5">
+        <v>3900</v>
+      </c>
+      <c r="W5">
+        <v>400</v>
+      </c>
+      <c r="X5">
+        <v>4000</v>
+      </c>
+      <c r="Y5">
+        <v>410</v>
+      </c>
+      <c r="Z5">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>4000</v>
+      </c>
+      <c r="E6">
+        <v>410</v>
+      </c>
+      <c r="F6">
+        <v>4100</v>
+      </c>
+      <c r="G6">
+        <v>420</v>
+      </c>
+      <c r="H6">
+        <v>4200</v>
+      </c>
+      <c r="I6">
+        <v>430</v>
+      </c>
+      <c r="J6">
+        <v>4300</v>
+      </c>
+      <c r="K6">
+        <v>440</v>
+      </c>
+      <c r="L6">
+        <v>4400</v>
+      </c>
+      <c r="M6">
+        <v>450</v>
+      </c>
+      <c r="N6">
+        <v>4500</v>
+      </c>
+      <c r="O6">
+        <v>460</v>
+      </c>
+      <c r="P6">
+        <v>4600</v>
+      </c>
+      <c r="Q6">
+        <v>470</v>
+      </c>
+      <c r="R6">
+        <v>4700</v>
+      </c>
+      <c r="S6">
+        <v>480</v>
+      </c>
+      <c r="T6">
+        <v>4800</v>
+      </c>
+      <c r="U6">
+        <v>490</v>
+      </c>
+      <c r="V6">
+        <v>4900</v>
+      </c>
+      <c r="W6">
+        <v>500</v>
+      </c>
+      <c r="X6">
+        <v>5000</v>
+      </c>
+      <c r="Y6">
+        <v>510</v>
+      </c>
+      <c r="Z6">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <v>510</v>
+      </c>
+      <c r="F7">
+        <v>5100</v>
+      </c>
+      <c r="G7">
+        <v>520</v>
+      </c>
+      <c r="H7">
+        <v>5200</v>
+      </c>
+      <c r="I7">
+        <v>530</v>
+      </c>
+      <c r="J7">
+        <v>5300</v>
+      </c>
+      <c r="K7">
+        <v>540</v>
+      </c>
+      <c r="L7">
+        <v>5400</v>
+      </c>
+      <c r="M7">
+        <v>550</v>
+      </c>
+      <c r="N7">
+        <v>5500</v>
+      </c>
+      <c r="O7">
+        <v>560</v>
+      </c>
+      <c r="P7">
+        <v>5600</v>
+      </c>
+      <c r="Q7">
+        <v>570</v>
+      </c>
+      <c r="R7">
+        <v>5700</v>
+      </c>
+      <c r="S7">
+        <v>580</v>
+      </c>
+      <c r="T7">
+        <v>5800</v>
+      </c>
+      <c r="U7">
+        <v>590</v>
+      </c>
+      <c r="V7">
+        <v>5900</v>
+      </c>
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7">
+        <v>6000</v>
+      </c>
+      <c r="Y7">
+        <v>610</v>
+      </c>
+      <c r="Z7">
+        <v>6100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>